<commit_message>
Oklahoma water rights update.
Oklahoma water rights update.  POU data and new readme.
</commit_message>
<xml_diff>
--- a/Oklahoma/WaterAllocation/OK_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Oklahoma/WaterAllocation/OK_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Oklahoma\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34532A9C-B0D8-4720-877B-B1951AB381EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6995435A-A040-4C2A-AC87-52D6C1BC07C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="5" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="300">
   <si>
     <t>Name</t>
   </si>
@@ -821,9 +821,6 @@
     <t>Concatenate OK with a counter</t>
   </si>
   <si>
-    <t>‘Unspecified</t>
-  </si>
-  <si>
     <t>LATITUDE</t>
   </si>
   <si>
@@ -887,15 +884,6 @@
     <t>1) State allocation data consist of two input csv files concatenated together.</t>
   </si>
   <si>
-    <t>2) I don't Rebecca Mitchell is the state contact name.  That seems to have been a default for a few states inputs.</t>
-  </si>
-  <si>
-    <t>3) Using OBJECTID as SiteNativeID, which may not be the best approach.  Should revisit this later after OK verification.</t>
-  </si>
-  <si>
-    <t>OBJECTID</t>
-  </si>
-  <si>
     <t>OBJECTID feels like a week entry.  May need to revisit this.</t>
   </si>
   <si>
@@ -924,6 +912,33 @@
   </si>
   <si>
     <t>bit</t>
+  </si>
+  <si>
+    <t>OwnerClassificationCV</t>
+  </si>
+  <si>
+    <t>Army (USA)</t>
+  </si>
+  <si>
+    <t>WSWC defined owner tag.</t>
+  </si>
+  <si>
+    <t>"Unspecified"</t>
+  </si>
+  <si>
+    <t>*Use cusotm WaDE ID</t>
+  </si>
+  <si>
+    <t>POD or POU (depends on input</t>
+  </si>
+  <si>
+    <t>2) Need to double check with OK on if they have a site ID value.</t>
+  </si>
+  <si>
+    <t>3) POU data shares similar columns.  Will just concatenate data together into one large input file.</t>
+  </si>
+  <si>
+    <t>Area of use: https://home-owrb.opendata.arcgis.com/datasets/areas-of-use?geometry=-109.718%2C33.749%2C-87.404%2C36.886</t>
   </si>
 </sst>
 </file>
@@ -1683,7 +1698,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1953,6 +1968,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2312,8 +2330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2330,7 +2348,7 @@
         <v>237</v>
       </c>
       <c r="B1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2346,12 +2364,17 @@
         <v>238</v>
       </c>
       <c r="B6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>277</v>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2359,17 +2382,17 @@
         <v>239</v>
       </c>
       <c r="B12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -3214,8 +3237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8BA2FE-2555-4166-A4DF-0203EE1C77D7}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3350,7 +3373,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="85" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>38</v>
@@ -3382,7 +3405,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>38</v>
@@ -3542,7 +3565,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="85" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>38</v>
@@ -3635,7 +3658,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3886,13 +3909,13 @@
         <v>38</v>
       </c>
       <c r="E9" s="73" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F9" s="73" t="s">
         <v>38</v>
       </c>
       <c r="G9" s="74" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="17">
@@ -3916,7 +3939,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="73" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F10" s="76" t="s">
         <v>38</v>
@@ -3953,8 +3976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E7F0DF-14BE-4BB8-BB6C-8815808B0B66}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4149,7 +4172,7 @@
         <v>38</v>
       </c>
       <c r="G7" s="49" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H7" s="82"/>
       <c r="I7" s="73" t="s">
@@ -4293,7 +4316,7 @@
       <c r="E12" s="73"/>
       <c r="F12" s="24"/>
       <c r="G12" s="25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H12" s="80"/>
       <c r="I12" s="22" t="s">
@@ -4323,7 +4346,7 @@
         <v>38</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H13" s="81"/>
       <c r="I13" s="18" t="s">
@@ -4353,7 +4376,7 @@
         <v>38</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H14" s="81"/>
       <c r="I14" s="18">
@@ -4425,7 +4448,7 @@
     </row>
     <row r="17" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>16</v>
@@ -4437,7 +4460,7 @@
         <v>38</v>
       </c>
       <c r="E17" s="65" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>38</v>
@@ -4447,7 +4470,7 @@
       </c>
       <c r="H17" s="86"/>
       <c r="I17" s="87" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="J17" s="86"/>
     </row>
@@ -4462,8 +4485,8 @@
       <c r="D18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="24" t="s">
-        <v>260</v>
+      <c r="E18" s="61" t="s">
+        <v>294</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>38</v>
@@ -4493,16 +4516,16 @@
         <v>38</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>38</v>
+        <v>295</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>38</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>284</v>
+        <v>38</v>
       </c>
       <c r="H19" s="79" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="I19" s="18">
         <v>3703994</v>
@@ -4555,13 +4578,13 @@
         <v>20</v>
       </c>
       <c r="E21" s="61" t="s">
-        <v>38</v>
+        <v>294</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="74" t="s">
-        <v>258</v>
+      <c r="G21" s="25" t="s">
+        <v>38</v>
       </c>
       <c r="H21" s="80"/>
       <c r="I21" s="18" t="s">
@@ -4642,10 +4665,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4966,7 +4989,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>38</v>
@@ -5030,7 +5053,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F13" s="44" t="s">
         <v>38</v>
@@ -5068,7 +5091,7 @@
         <v>38</v>
       </c>
       <c r="G14" s="49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H14" s="38" t="s">
         <v>38</v>
@@ -5306,7 +5329,7 @@
     </row>
     <row r="22" spans="1:10" s="37" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>69</v>
@@ -5327,7 +5350,7 @@
         <v>38</v>
       </c>
       <c r="H22" s="84" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I22" s="18">
         <v>1</v>
@@ -5356,7 +5379,7 @@
         <v>38</v>
       </c>
       <c r="G23" s="49" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H23" s="38" t="s">
         <v>38</v>
@@ -5388,7 +5411,7 @@
         <v>38</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H24" s="38" t="s">
         <v>38</v>
@@ -5420,7 +5443,7 @@
         <v>38</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H25" s="38" t="s">
         <v>38</v>
@@ -5452,7 +5475,7 @@
         <v>38</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H26" s="38" t="s">
         <v>38</v>
@@ -5580,7 +5603,7 @@
         <v>38</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H30" s="38" t="s">
         <v>38</v>
@@ -5594,7 +5617,7 @@
     </row>
     <row r="31" spans="1:10" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>69</v>
@@ -5612,7 +5635,7 @@
         <v>38</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H31" s="38" t="s">
         <v>38</v>
@@ -5644,7 +5667,7 @@
         <v>38</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H32" s="38" t="s">
         <v>38</v>
@@ -5656,7 +5679,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>101</v>
       </c>
@@ -5688,7 +5711,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>98</v>
       </c>
@@ -5720,7 +5743,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="52" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" s="52" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>100</v>
       </c>
@@ -5752,7 +5775,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="52" t="s">
         <v>155</v>
       </c>
@@ -5784,12 +5807,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="88" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B37" s="53" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C37" s="54" t="s">
         <v>18</v>
@@ -5810,7 +5833,7 @@
       <c r="I37" s="90"/>
       <c r="J37" s="91"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>82</v>
       </c>
@@ -5842,7 +5865,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>90</v>
       </c>
@@ -5874,7 +5897,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>91</v>
       </c>
@@ -5904,7 +5927,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>99</v>
       </c>
@@ -5936,7 +5959,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>96</v>
       </c>
@@ -5968,50 +5991,50 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>89</v>
+        <v>291</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="F43" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="G43" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="D43" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="92"/>
       <c r="H43" s="38" t="s">
         <v>38</v>
       </c>
       <c r="I43" s="67" t="s">
-        <v>38</v>
+        <v>292</v>
       </c>
       <c r="J43" s="63" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E44" s="24" t="s">
         <v>240</v>
@@ -6025,80 +6048,112 @@
       <c r="H44" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="I44" s="18" t="s">
+      <c r="I44" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" s="63" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="F45" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="H45" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J44" s="64" t="s">
+      <c r="J45" s="64" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="52" t="s">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="B45" s="53" t="s">
+      <c r="B46" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="C45" s="54" t="s">
+      <c r="C46" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="56" t="s">
+      <c r="D46" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="24" t="s">
+      <c r="E46" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="F46" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="I46" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="F45" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="G45" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="H45" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="I45" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="J45" s="63" t="s">
+      <c r="J46" s="63" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B47" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" s="24" t="s">
+      <c r="D47" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="F46" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="G46" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="H46" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="I46" s="18" t="s">
+      <c r="F47" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="I47" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J46" s="63" t="s">
+      <c r="J47" s="63" t="s">
         <v>211</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:J46">
-    <sortCondition ref="A14:A46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:J47">
+    <sortCondition ref="A14:A47"/>
   </sortState>
   <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
OKwr & WAwr update.
OKwr & WAwr update.  New m-m relationship between sites and water sources.  New group by statement for allocations.  Added geometry for POU sites.
</commit_message>
<xml_diff>
--- a/Oklahoma/WaterAllocation/OK_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Oklahoma/WaterAllocation/OK_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Oklahoma\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6995435A-A040-4C2A-AC87-52D6C1BC07C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9491E961-A9A6-4B55-9DF1-44F461B562B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="5" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="300">
   <si>
     <t>Name</t>
   </si>
@@ -788,18 +788,9 @@
     <t>Water Allocation</t>
   </si>
   <si>
-    <t>OWRB_Water Rights</t>
-  </si>
-  <si>
     <t>Oklahoma Water Rights</t>
   </si>
   <si>
-    <t>OWRB_Allocation All</t>
-  </si>
-  <si>
-    <t>OWRB</t>
-  </si>
-  <si>
     <t>Oklahoma Water Resources Board</t>
   </si>
   <si>
@@ -812,15 +803,9 @@
     <t>OK</t>
   </si>
   <si>
-    <t>Concatenate OK with a counter.</t>
-  </si>
-  <si>
     <t>WATER</t>
   </si>
   <si>
-    <t>Concatenate OK with a counter</t>
-  </si>
-  <si>
     <t>LATITUDE</t>
   </si>
   <si>
@@ -939,6 +924,21 @@
   </si>
   <si>
     <t>Area of use: https://home-owrb.opendata.arcgis.com/datasets/areas-of-use?geometry=-109.718%2C33.749%2C-87.404%2C36.886</t>
+  </si>
+  <si>
+    <t>OKwr_M1</t>
+  </si>
+  <si>
+    <t>OKwr_V1</t>
+  </si>
+  <si>
+    <t>OKwr_O1</t>
+  </si>
+  <si>
+    <t>OKwr_WS + counter</t>
+  </si>
+  <si>
+    <t>OKwr_S + counter</t>
   </si>
 </sst>
 </file>
@@ -1698,7 +1698,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1971,6 +1971,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2348,7 +2351,7 @@
         <v>237</v>
       </c>
       <c r="B1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2356,7 +2359,7 @@
         <v>245</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2364,17 +2367,17 @@
         <v>238</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2382,17 +2385,17 @@
         <v>239</v>
       </c>
       <c r="B12" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -2432,7 +2435,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2535,7 +2538,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>249</v>
+        <v>295</v>
       </c>
       <c r="F4" s="44" t="s">
         <v>38</v>
@@ -2725,7 +2728,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>38</v>
@@ -2821,7 +2824,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2918,7 +2921,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>251</v>
+        <v>296</v>
       </c>
       <c r="F4" s="44" t="s">
         <v>38</v>
@@ -3238,7 +3241,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3341,7 +3344,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>252</v>
+        <v>297</v>
       </c>
       <c r="F4" s="44" t="s">
         <v>38</v>
@@ -3373,7 +3376,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="85" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>38</v>
@@ -3405,7 +3408,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>38</v>
@@ -3437,7 +3440,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="85" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>38</v>
@@ -3469,7 +3472,7 @@
         <v>38</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>38</v>
@@ -3533,7 +3536,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>38</v>
@@ -3565,7 +3568,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="85" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>38</v>
@@ -3597,7 +3600,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>38</v>
@@ -3658,7 +3661,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3759,7 +3762,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>257</v>
+        <v>298</v>
       </c>
       <c r="F4" s="44" t="s">
         <v>38</v>
@@ -3909,13 +3912,13 @@
         <v>38</v>
       </c>
       <c r="E9" s="73" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F9" s="73" t="s">
         <v>38</v>
       </c>
       <c r="G9" s="74" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="17">
@@ -3939,13 +3942,13 @@
         <v>20</v>
       </c>
       <c r="E10" s="73" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F10" s="76" t="s">
         <v>38</v>
       </c>
       <c r="G10" s="74" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="H10" s="23"/>
       <c r="I10" s="17" t="s">
@@ -3976,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E7F0DF-14BE-4BB8-BB6C-8815808B0B66}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4076,7 +4079,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>259</v>
+        <v>299</v>
       </c>
       <c r="F4" s="44" t="s">
         <v>38</v>
@@ -4172,7 +4175,7 @@
         <v>38</v>
       </c>
       <c r="G7" s="49" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="H7" s="82"/>
       <c r="I7" s="73" t="s">
@@ -4316,7 +4319,7 @@
       <c r="E12" s="73"/>
       <c r="F12" s="24"/>
       <c r="G12" s="25" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="H12" s="80"/>
       <c r="I12" s="22" t="s">
@@ -4346,7 +4349,7 @@
         <v>38</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H13" s="81"/>
       <c r="I13" s="18" t="s">
@@ -4376,7 +4379,7 @@
         <v>38</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="H14" s="81"/>
       <c r="I14" s="18">
@@ -4448,7 +4451,7 @@
     </row>
     <row r="17" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>16</v>
@@ -4460,7 +4463,7 @@
         <v>38</v>
       </c>
       <c r="E17" s="65" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>38</v>
@@ -4470,7 +4473,7 @@
       </c>
       <c r="H17" s="86"/>
       <c r="I17" s="87" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="J17" s="86"/>
     </row>
@@ -4486,7 +4489,7 @@
         <v>38</v>
       </c>
       <c r="E18" s="61" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>38</v>
@@ -4516,7 +4519,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>38</v>
@@ -4525,7 +4528,7 @@
         <v>38</v>
       </c>
       <c r="H19" s="79" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I19" s="18">
         <v>3703994</v>
@@ -4578,7 +4581,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="61" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>38</v>
@@ -4608,7 +4611,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>38</v>
@@ -4667,8 +4670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4925,7 +4928,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="59" t="s">
-        <v>249</v>
+        <v>295</v>
       </c>
       <c r="F9" s="34" t="s">
         <v>38</v>
@@ -4957,7 +4960,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="61" t="s">
-        <v>252</v>
+        <v>297</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>38</v>
@@ -4989,7 +4992,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>38</v>
@@ -5021,7 +5024,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>251</v>
+        <v>296</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>38</v>
@@ -5053,7 +5056,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="F13" s="44" t="s">
         <v>38</v>
@@ -5091,7 +5094,7 @@
         <v>38</v>
       </c>
       <c r="G14" s="49" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="H14" s="38" t="s">
         <v>38</v>
@@ -5329,7 +5332,7 @@
     </row>
     <row r="22" spans="1:10" s="37" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>69</v>
@@ -5350,7 +5353,7 @@
         <v>38</v>
       </c>
       <c r="H22" s="84" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="I22" s="18">
         <v>1</v>
@@ -5379,7 +5382,7 @@
         <v>38</v>
       </c>
       <c r="G23" s="49" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="H23" s="38" t="s">
         <v>38</v>
@@ -5411,7 +5414,7 @@
         <v>38</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H24" s="38" t="s">
         <v>38</v>
@@ -5443,7 +5446,7 @@
         <v>38</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="H25" s="38" t="s">
         <v>38</v>
@@ -5475,7 +5478,7 @@
         <v>38</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="H26" s="38" t="s">
         <v>38</v>
@@ -5603,7 +5606,7 @@
         <v>38</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H30" s="38" t="s">
         <v>38</v>
@@ -5617,7 +5620,7 @@
     </row>
     <row r="31" spans="1:10" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>69</v>
@@ -5635,7 +5638,7 @@
         <v>38</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="H31" s="38" t="s">
         <v>38</v>
@@ -5667,7 +5670,7 @@
         <v>38</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H32" s="38" t="s">
         <v>38</v>
@@ -5788,8 +5791,8 @@
       <c r="D36" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="24" t="s">
-        <v>240</v>
+      <c r="E36" s="93">
+        <v>44650</v>
       </c>
       <c r="F36" s="34" t="s">
         <v>38</v>
@@ -5809,10 +5812,10 @@
     </row>
     <row r="37" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="88" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B37" s="53" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C37" s="54" t="s">
         <v>18</v>
@@ -5993,7 +5996,7 @@
     </row>
     <row r="43" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>34</v>
@@ -6011,10 +6014,10 @@
         <v>38</v>
       </c>
       <c r="I43" s="67" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="J43" s="63" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>

</xml_diff>